<commit_message>
Add AExcelParser class -Add AExcelParser class to create parser parsing excel file. -Change parental class of CExcelParser from AParser to AExcelParser. -Update format of table to define the function.
</commit_message>
<xml_diff>
--- a/doc/template_for_CStubMk.xlsx
+++ b/doc/template_for_CStubMk.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1"/>
@@ -90,6 +90,22 @@
   </si>
   <si>
     <t>WORD</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>lang</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ver.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0.1.0</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -97,7 +113,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +143,13 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Meiryo UI"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -328,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -343,7 +366,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -352,18 +378,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -673,15 +697,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I3"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:I10"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.25" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.25" style="1"/>
+    <col min="1" max="1" width="4.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.25" style="1" bestFit="1" customWidth="1"/>
@@ -693,52 +717,387 @@
     <col min="10" max="16384" width="2.25" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="14" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="16"/>
-    </row>
-    <row r="3" spans="2:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="17"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="19" t="s">
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="17"/>
+    </row>
+    <row r="4" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="20"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I4" s="15" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28" s="5"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B29" s="5"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" s="5"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" s="5"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="7"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B32" s="5"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="7"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B33" s="5"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="7"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B34" s="5"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="7"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B35" s="5"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="7"/>
+    </row>
+    <row r="36" spans="2:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="8"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -768,40 +1127,40 @@
   <sheetData>
     <row r="1" spans="2:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="2:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="17"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="15" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add parameter to Param class. -Add member named "Mode", its data type is AccessMode in enum, representing the access mode, input, output or both. -Add member method to convert string into AccessMode data type. -Add operation to get from table in format, convert, and set into param object. -Update template.
</commit_message>
<xml_diff>
--- a/doc/template_for_CStubMk.xlsx
+++ b/doc/template_for_CStubMk.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1"/>
@@ -106,6 +106,10 @@
   </si>
   <si>
     <t>0.1.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mode(in/out/both)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -351,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -372,6 +376,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -387,7 +395,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -697,11 +704,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.25" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -714,64 +719,69 @@
     <col min="7" max="7" width="9.125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.25" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="2.25" style="1"/>
+    <col min="10" max="10" width="19.5" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="2.25" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+    <row r="2" spans="1:10" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="19" t="s">
+    <row r="3" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="17"/>
-    </row>
-    <row r="4" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="20"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="14" t="s">
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="19"/>
+    </row>
+    <row r="4" spans="1:10" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="22"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="16" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -779,9 +789,10 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I5" s="3"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -789,9 +800,10 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I6" s="6"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -799,9 +811,10 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I7" s="6"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8" s="5"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -809,9 +822,10 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I8" s="6"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -819,9 +833,10 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I9" s="6"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -829,9 +844,10 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I10" s="6"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -839,9 +855,10 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I11" s="6"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -849,9 +866,10 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I12" s="6"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -859,9 +877,10 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I13" s="6"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -869,9 +888,10 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I14" s="6"/>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -879,9 +899,10 @@
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I15" s="6"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -889,9 +910,10 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I16" s="6"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -899,9 +921,10 @@
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I17" s="6"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="5"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -909,9 +932,10 @@
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
-      <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I18" s="6"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -919,9 +943,10 @@
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
-      <c r="I19" s="7"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I19" s="6"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="5"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -929,9 +954,10 @@
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
-      <c r="I20" s="7"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I20" s="6"/>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -939,9 +965,10 @@
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
-      <c r="I21" s="7"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I21" s="6"/>
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="5"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -949,9 +976,10 @@
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
-      <c r="I22" s="7"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I22" s="6"/>
+      <c r="J22" s="7"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="5"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -959,9 +987,10 @@
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
-      <c r="I23" s="7"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I23" s="6"/>
+      <c r="J23" s="7"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B24" s="5"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -969,9 +998,10 @@
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
-      <c r="I24" s="7"/>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I24" s="6"/>
+      <c r="J24" s="7"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -979,9 +1009,10 @@
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
-      <c r="I25" s="7"/>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I25" s="6"/>
+      <c r="J25" s="7"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B26" s="5"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -989,9 +1020,10 @@
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
-      <c r="I26" s="7"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I26" s="6"/>
+      <c r="J26" s="7"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B27" s="5"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -999,9 +1031,10 @@
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
-      <c r="I27" s="7"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I27" s="6"/>
+      <c r="J27" s="7"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -1009,9 +1042,10 @@
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
-      <c r="I28" s="7"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I28" s="6"/>
+      <c r="J28" s="7"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -1019,9 +1053,10 @@
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
-      <c r="I29" s="7"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I29" s="6"/>
+      <c r="J29" s="7"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B30" s="5"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -1029,9 +1064,10 @@
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
-      <c r="I30" s="7"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I30" s="6"/>
+      <c r="J30" s="7"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B31" s="5"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
@@ -1039,9 +1075,10 @@
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
-      <c r="I31" s="7"/>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I31" s="6"/>
+      <c r="J31" s="7"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B32" s="5"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
@@ -1049,9 +1086,10 @@
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
-      <c r="I32" s="7"/>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I32" s="6"/>
+      <c r="J32" s="7"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B33" s="5"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
@@ -1059,9 +1097,10 @@
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
-      <c r="I33" s="7"/>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I33" s="6"/>
+      <c r="J33" s="7"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B34" s="5"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
@@ -1069,9 +1108,10 @@
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
-      <c r="I34" s="7"/>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I34" s="6"/>
+      <c r="J34" s="7"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B35" s="5"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
@@ -1079,9 +1119,10 @@
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
-      <c r="I35" s="7"/>
-    </row>
-    <row r="36" spans="2:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I35" s="6"/>
+      <c r="J35" s="7"/>
+    </row>
+    <row r="36" spans="2:10" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="8"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
@@ -1089,11 +1130,12 @@
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
-      <c r="I36" s="10"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="F3:J3"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="D3:D4"/>
@@ -1127,30 +1169,30 @@
   <sheetData>
     <row r="1" spans="2:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="17"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="2:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="20"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
       <c r="F3" s="14" t="s">
         <v>0</v>
       </c>

</xml_diff>